<commit_message>
Diet scripts and plots updated for the hake and energetics
</commit_message>
<xml_diff>
--- a/Length Weight/TTR_LengthWeight.xlsx
+++ b/Length Weight/TTR_LengthWeight.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="16155"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="16155" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="biblio" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Bottlenose dolphin (Tursiops truncatus)</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>Ridgway and Fenner, 1982</t>
+  </si>
+  <si>
+    <t>Wells and Scott, 1999</t>
+  </si>
+  <si>
+    <t>Pierce et al., 2005</t>
+  </si>
+  <si>
+    <t>log W = 5.597 + 3.2692 log L (R2=0.711)</t>
+  </si>
+  <si>
+    <t>Pierce, G.J., Santos, M.B., Learmonth, J.A., Smeenk, C., Addink, M., García Hartmann, M., Boon, J.P., Zegers, B., Mets, A., Ridoux, V., Caurant, F., Bustamante, P., Lahaye, V., Guerra, A., González, A., López, A., Alonso, J.M., Rogan, E., Murphy, S., Van Canneyt, O., Dabin,W., Spitz, J., Doemus, G., Meynier, L., 2005. Bioaccumulation of persistent organic pollutants in small cetaceans in European waters: transport pathways and impact on reproduction. Final Report to the European Commission's Directorate General for Research on Project EVK3-2000-00027.</t>
   </si>
 </sst>
 </file>
@@ -78,8 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -491,12 +508,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A4:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Script de talla peso y excel con los datos para Gadget actualizados
</commit_message>
<xml_diff>
--- a/Length Weight/TTR_LengthWeight.xlsx
+++ b/Length Weight/TTR_LengthWeight.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="16155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="16155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="biblio" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="len-wei Gadget" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="156">
   <si>
     <t>Bottlenose dolphin (Tursiops truncatus)</t>
   </si>
@@ -58,6 +58,432 @@
   </si>
   <si>
     <t>Pierce, G.J., Santos, M.B., Learmonth, J.A., Smeenk, C., Addink, M., García Hartmann, M., Boon, J.P., Zegers, B., Mets, A., Ridoux, V., Caurant, F., Bustamante, P., Lahaye, V., Guerra, A., González, A., López, A., Alonso, J.M., Rogan, E., Murphy, S., Van Canneyt, O., Dabin,W., Spitz, J., Doemus, G., Meynier, L., 2005. Bioaccumulation of persistent organic pollutants in small cetaceans in European waters: transport pathways and impact on reproduction. Final Report to the European Commission's Directorate General for Research on Project EVK3-2000-00027.</t>
+  </si>
+  <si>
+    <t>len110</t>
+  </si>
+  <si>
+    <t>len111</t>
+  </si>
+  <si>
+    <t>len112</t>
+  </si>
+  <si>
+    <t>len113</t>
+  </si>
+  <si>
+    <t>len114</t>
+  </si>
+  <si>
+    <t>len115</t>
+  </si>
+  <si>
+    <t>len116</t>
+  </si>
+  <si>
+    <t>len117</t>
+  </si>
+  <si>
+    <t>len118</t>
+  </si>
+  <si>
+    <t>len119</t>
+  </si>
+  <si>
+    <t>len120</t>
+  </si>
+  <si>
+    <t>len121</t>
+  </si>
+  <si>
+    <t>len122</t>
+  </si>
+  <si>
+    <t>len123</t>
+  </si>
+  <si>
+    <t>len124</t>
+  </si>
+  <si>
+    <t>len125</t>
+  </si>
+  <si>
+    <t>len126</t>
+  </si>
+  <si>
+    <t>len127</t>
+  </si>
+  <si>
+    <t>len128</t>
+  </si>
+  <si>
+    <t>len129</t>
+  </si>
+  <si>
+    <t>len130</t>
+  </si>
+  <si>
+    <t>len131</t>
+  </si>
+  <si>
+    <t>len132</t>
+  </si>
+  <si>
+    <t>len133</t>
+  </si>
+  <si>
+    <t>len134</t>
+  </si>
+  <si>
+    <t>len135</t>
+  </si>
+  <si>
+    <t>len136</t>
+  </si>
+  <si>
+    <t>len137</t>
+  </si>
+  <si>
+    <t>len138</t>
+  </si>
+  <si>
+    <t>len139</t>
+  </si>
+  <si>
+    <t>len140</t>
+  </si>
+  <si>
+    <t>len141</t>
+  </si>
+  <si>
+    <t>len142</t>
+  </si>
+  <si>
+    <t>len143</t>
+  </si>
+  <si>
+    <t>len144</t>
+  </si>
+  <si>
+    <t>len145</t>
+  </si>
+  <si>
+    <t>len146</t>
+  </si>
+  <si>
+    <t>len147</t>
+  </si>
+  <si>
+    <t>len148</t>
+  </si>
+  <si>
+    <t>len149</t>
+  </si>
+  <si>
+    <t>len150</t>
+  </si>
+  <si>
+    <t>len151</t>
+  </si>
+  <si>
+    <t>len152</t>
+  </si>
+  <si>
+    <t>len153</t>
+  </si>
+  <si>
+    <t>len154</t>
+  </si>
+  <si>
+    <t>len155</t>
+  </si>
+  <si>
+    <t>len156</t>
+  </si>
+  <si>
+    <t>len157</t>
+  </si>
+  <si>
+    <t>len158</t>
+  </si>
+  <si>
+    <t>len159</t>
+  </si>
+  <si>
+    <t>len160</t>
+  </si>
+  <si>
+    <t>len161</t>
+  </si>
+  <si>
+    <t>len162</t>
+  </si>
+  <si>
+    <t>len163</t>
+  </si>
+  <si>
+    <t>len164</t>
+  </si>
+  <si>
+    <t>len165</t>
+  </si>
+  <si>
+    <t>len166</t>
+  </si>
+  <si>
+    <t>len167</t>
+  </si>
+  <si>
+    <t>len168</t>
+  </si>
+  <si>
+    <t>len169</t>
+  </si>
+  <si>
+    <t>len170</t>
+  </si>
+  <si>
+    <t>len171</t>
+  </si>
+  <si>
+    <t>len172</t>
+  </si>
+  <si>
+    <t>len173</t>
+  </si>
+  <si>
+    <t>len174</t>
+  </si>
+  <si>
+    <t>len175</t>
+  </si>
+  <si>
+    <t>len176</t>
+  </si>
+  <si>
+    <t>len177</t>
+  </si>
+  <si>
+    <t>len178</t>
+  </si>
+  <si>
+    <t>len179</t>
+  </si>
+  <si>
+    <t>len180</t>
+  </si>
+  <si>
+    <t>len181</t>
+  </si>
+  <si>
+    <t>len182</t>
+  </si>
+  <si>
+    <t>len183</t>
+  </si>
+  <si>
+    <t>len184</t>
+  </si>
+  <si>
+    <t>len185</t>
+  </si>
+  <si>
+    <t>len186</t>
+  </si>
+  <si>
+    <t>len187</t>
+  </si>
+  <si>
+    <t>len188</t>
+  </si>
+  <si>
+    <t>len189</t>
+  </si>
+  <si>
+    <t>len190</t>
+  </si>
+  <si>
+    <t>len191</t>
+  </si>
+  <si>
+    <t>len192</t>
+  </si>
+  <si>
+    <t>len193</t>
+  </si>
+  <si>
+    <t>len194</t>
+  </si>
+  <si>
+    <t>len195</t>
+  </si>
+  <si>
+    <t>len196</t>
+  </si>
+  <si>
+    <t>len197</t>
+  </si>
+  <si>
+    <t>len198</t>
+  </si>
+  <si>
+    <t>len199</t>
+  </si>
+  <si>
+    <t>len200</t>
+  </si>
+  <si>
+    <t>len201</t>
+  </si>
+  <si>
+    <t>len202</t>
+  </si>
+  <si>
+    <t>len203</t>
+  </si>
+  <si>
+    <t>len204</t>
+  </si>
+  <si>
+    <t>len205</t>
+  </si>
+  <si>
+    <t>len206</t>
+  </si>
+  <si>
+    <t>len207</t>
+  </si>
+  <si>
+    <t>len208</t>
+  </si>
+  <si>
+    <t>len209</t>
+  </si>
+  <si>
+    <t>len210</t>
+  </si>
+  <si>
+    <t>len211</t>
+  </si>
+  <si>
+    <t>len212</t>
+  </si>
+  <si>
+    <t>len213</t>
+  </si>
+  <si>
+    <t>len214</t>
+  </si>
+  <si>
+    <t>len215</t>
+  </si>
+  <si>
+    <t>len216</t>
+  </si>
+  <si>
+    <t>len217</t>
+  </si>
+  <si>
+    <t>len218</t>
+  </si>
+  <si>
+    <t>len219</t>
+  </si>
+  <si>
+    <t>len220</t>
+  </si>
+  <si>
+    <t>len221</t>
+  </si>
+  <si>
+    <t>len222</t>
+  </si>
+  <si>
+    <t>len223</t>
+  </si>
+  <si>
+    <t>len224</t>
+  </si>
+  <si>
+    <t>len225</t>
+  </si>
+  <si>
+    <t>len226</t>
+  </si>
+  <si>
+    <t>len227</t>
+  </si>
+  <si>
+    <t>len228</t>
+  </si>
+  <si>
+    <t>len229</t>
+  </si>
+  <si>
+    <t>len230</t>
+  </si>
+  <si>
+    <t>len231</t>
+  </si>
+  <si>
+    <t>len232</t>
+  </si>
+  <si>
+    <t>len233</t>
+  </si>
+  <si>
+    <t>len234</t>
+  </si>
+  <si>
+    <t>len235</t>
+  </si>
+  <si>
+    <t>len236</t>
+  </si>
+  <si>
+    <t>len237</t>
+  </si>
+  <si>
+    <t>len238</t>
+  </si>
+  <si>
+    <t>len239</t>
+  </si>
+  <si>
+    <t>len240</t>
+  </si>
+  <si>
+    <t>len241</t>
+  </si>
+  <si>
+    <t>len242</t>
+  </si>
+  <si>
+    <t>len243</t>
+  </si>
+  <si>
+    <t>len244</t>
+  </si>
+  <si>
+    <t>len245</t>
+  </si>
+  <si>
+    <t>len246</t>
+  </si>
+  <si>
+    <t>len247</t>
+  </si>
+  <si>
+    <t>len248</t>
+  </si>
+  <si>
+    <t>len249</t>
+  </si>
+  <si>
+    <t>len250</t>
+  </si>
+  <si>
+    <t>Following Wells and Scott, 1999 for all bottlenose dolphins</t>
   </si>
 </sst>
 </file>
@@ -93,10 +519,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +823,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -510,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -544,12 +973,1574 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C143"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="3" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
+        <v>110.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>24.685580000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
+        <v>111.5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>25.058759999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>25.437570000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
+        <v>113.5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>25.822120000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3">
+        <v>114.5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>26.21247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
+        <v>115.5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>26.608730000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3">
+        <v>116.5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>27.01098</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3">
+        <v>117.5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>27.4193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3">
+        <v>118.5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>27.83381</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3">
+        <v>119.5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>28.254570000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3">
+        <v>120.5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>28.681699999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3">
+        <v>121.5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>29.115290000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3">
+        <v>122.5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>29.555430000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3">
+        <v>123.5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>30.002220000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3">
+        <v>124.5</v>
+      </c>
+      <c r="C17" s="3">
+        <v>30.455770000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3">
+        <v>125.5</v>
+      </c>
+      <c r="C18" s="3">
+        <v>30.916170000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3">
+        <v>126.5</v>
+      </c>
+      <c r="C19" s="3">
+        <v>31.38353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3">
+        <v>127.5</v>
+      </c>
+      <c r="C20" s="3">
+        <v>31.857959999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3">
+        <v>128.5</v>
+      </c>
+      <c r="C21" s="3">
+        <v>32.339570000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="3">
+        <v>129.5</v>
+      </c>
+      <c r="C22" s="3">
+        <v>32.828449999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="3">
+        <v>130.5</v>
+      </c>
+      <c r="C23" s="3">
+        <v>33.324719999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="3">
+        <v>131.5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>33.828490000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="3">
+        <v>132.5</v>
+      </c>
+      <c r="C25" s="3">
+        <v>34.339880000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="3">
+        <v>133.5</v>
+      </c>
+      <c r="C26" s="3">
+        <v>34.859000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="3">
+        <v>134.5</v>
+      </c>
+      <c r="C27" s="3">
+        <v>35.38597</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="3">
+        <v>135.5</v>
+      </c>
+      <c r="C28" s="3">
+        <v>35.920909999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="3">
+        <v>136.5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>36.463929999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="3">
+        <v>137.5</v>
+      </c>
+      <c r="C30" s="3">
+        <v>37.015160000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="3">
+        <v>138.5</v>
+      </c>
+      <c r="C31" s="3">
+        <v>37.574719999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="3">
+        <v>139.5</v>
+      </c>
+      <c r="C32" s="3">
+        <v>38.142740000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="3">
+        <v>140.5</v>
+      </c>
+      <c r="C33" s="3">
+        <v>38.719349999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="3">
+        <v>141.5</v>
+      </c>
+      <c r="C34" s="3">
+        <v>39.304679999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="3">
+        <v>142.5</v>
+      </c>
+      <c r="C35" s="3">
+        <v>39.898850000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="3">
+        <v>143.5</v>
+      </c>
+      <c r="C36" s="3">
+        <v>40.502009999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="3">
+        <v>144.5</v>
+      </c>
+      <c r="C37" s="3">
+        <v>41.114280000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="3">
+        <v>145.5</v>
+      </c>
+      <c r="C38" s="3">
+        <v>41.735810000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="3">
+        <v>146.5</v>
+      </c>
+      <c r="C39" s="3">
+        <v>42.36674</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="3">
+        <v>147.5</v>
+      </c>
+      <c r="C40" s="3">
+        <v>43.007199999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="3">
+        <v>148.5</v>
+      </c>
+      <c r="C41" s="3">
+        <v>43.657350000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="3">
+        <v>149.5</v>
+      </c>
+      <c r="C42" s="3">
+        <v>44.317320000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="3">
+        <v>150.5</v>
+      </c>
+      <c r="C43" s="3">
+        <v>44.987270000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="3">
+        <v>151.5</v>
+      </c>
+      <c r="C44" s="3">
+        <v>45.667349999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="3">
+        <v>152.5</v>
+      </c>
+      <c r="C45" s="3">
+        <v>46.357709999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="3">
+        <v>153.5</v>
+      </c>
+      <c r="C46" s="3">
+        <v>47.058500000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="3">
+        <v>154.5</v>
+      </c>
+      <c r="C47" s="3">
+        <v>47.769889999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="3">
+        <v>155.5</v>
+      </c>
+      <c r="C48" s="3">
+        <v>48.492040000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="3">
+        <v>156.5</v>
+      </c>
+      <c r="C49" s="3">
+        <v>49.225099999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="3">
+        <v>157.5</v>
+      </c>
+      <c r="C50" s="3">
+        <v>49.969239999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="3">
+        <v>158.5</v>
+      </c>
+      <c r="C51" s="3">
+        <v>50.724629999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="3">
+        <v>159.5</v>
+      </c>
+      <c r="C52" s="3">
+        <v>51.491439999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="3">
+        <v>160.5</v>
+      </c>
+      <c r="C53" s="3">
+        <v>52.269849999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="3">
+        <v>161.5</v>
+      </c>
+      <c r="C54" s="3">
+        <v>53.060020000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="3">
+        <v>162.5</v>
+      </c>
+      <c r="C55" s="3">
+        <v>53.862130000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="3">
+        <v>163.5</v>
+      </c>
+      <c r="C56" s="3">
+        <v>54.676369999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="3">
+        <v>164.5</v>
+      </c>
+      <c r="C57" s="3">
+        <v>55.502920000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="3">
+        <v>165.5</v>
+      </c>
+      <c r="C58" s="3">
+        <v>56.341970000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="3">
+        <v>166.5</v>
+      </c>
+      <c r="C59" s="3">
+        <v>57.1937</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="3">
+        <v>167.5</v>
+      </c>
+      <c r="C60" s="3">
+        <v>58.058300000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="3">
+        <v>168.5</v>
+      </c>
+      <c r="C61" s="3">
+        <v>58.935980000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="3">
+        <v>169.5</v>
+      </c>
+      <c r="C62" s="3">
+        <v>59.826920000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="3">
+        <v>170.5</v>
+      </c>
+      <c r="C63" s="3">
+        <v>60.73133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="3">
+        <v>171.5</v>
+      </c>
+      <c r="C64" s="3">
+        <v>61.649410000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="3">
+        <v>172.5</v>
+      </c>
+      <c r="C65" s="3">
+        <v>62.581380000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="3">
+        <v>173.5</v>
+      </c>
+      <c r="C66" s="3">
+        <v>63.527430000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="3">
+        <v>174.5</v>
+      </c>
+      <c r="C67" s="3">
+        <v>64.487780000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="3">
+        <v>175.5</v>
+      </c>
+      <c r="C68" s="3">
+        <v>65.462649999999996</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="3">
+        <v>176.5</v>
+      </c>
+      <c r="C69" s="3">
+        <v>66.452259999999995</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="3">
+        <v>177.5</v>
+      </c>
+      <c r="C70" s="3">
+        <v>67.456819999999993</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" s="3">
+        <v>178.5</v>
+      </c>
+      <c r="C71" s="3">
+        <v>68.476579999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" s="3">
+        <v>179.5</v>
+      </c>
+      <c r="C72" s="3">
+        <v>69.511750000000006</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" s="3">
+        <v>180.5</v>
+      </c>
+      <c r="C73" s="3">
+        <v>70.562569999999994</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="3">
+        <v>181.5</v>
+      </c>
+      <c r="C74" s="3">
+        <v>71.629270000000005</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="3">
+        <v>182.5</v>
+      </c>
+      <c r="C75" s="3">
+        <v>72.712100000000007</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="3">
+        <v>183.5</v>
+      </c>
+      <c r="C76" s="3">
+        <v>73.811300000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" s="3">
+        <v>184.5</v>
+      </c>
+      <c r="C77" s="3">
+        <v>74.927109999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="3">
+        <v>185.5</v>
+      </c>
+      <c r="C78" s="3">
+        <v>76.059799999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="3">
+        <v>186.5</v>
+      </c>
+      <c r="C79" s="3">
+        <v>77.209599999999995</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" s="3">
+        <v>187.5</v>
+      </c>
+      <c r="C80" s="3">
+        <v>78.37679</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" s="3">
+        <v>188.5</v>
+      </c>
+      <c r="C81" s="3">
+        <v>79.561620000000005</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="3">
+        <v>189.5</v>
+      </c>
+      <c r="C82" s="3">
+        <v>80.76437</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="3">
+        <v>190.5</v>
+      </c>
+      <c r="C83" s="3">
+        <v>81.985290000000006</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84" s="3">
+        <v>191.5</v>
+      </c>
+      <c r="C84" s="3">
+        <v>83.224670000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" s="3">
+        <v>192.5</v>
+      </c>
+      <c r="C85" s="3">
+        <v>84.482789999999994</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" s="3">
+        <v>193.5</v>
+      </c>
+      <c r="C86" s="3">
+        <v>85.759929999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" s="3">
+        <v>194.5</v>
+      </c>
+      <c r="C87" s="3">
+        <v>87.056370000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" s="3">
+        <v>195.5</v>
+      </c>
+      <c r="C88" s="3">
+        <v>88.372420000000005</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89" s="3">
+        <v>196.5</v>
+      </c>
+      <c r="C89" s="3">
+        <v>89.708349999999996</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="3">
+        <v>197.5</v>
+      </c>
+      <c r="C90" s="3">
+        <v>91.064490000000006</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" s="3">
+        <v>198.5</v>
+      </c>
+      <c r="C91" s="3">
+        <v>92.441119999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" s="3">
+        <v>199.5</v>
+      </c>
+      <c r="C92" s="3">
+        <v>93.838570000000004</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" s="3">
+        <v>200.5</v>
+      </c>
+      <c r="C93" s="3">
+        <v>95.257140000000007</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94" s="3">
+        <v>201.5</v>
+      </c>
+      <c r="C94" s="3">
+        <v>96.697149999999993</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" s="3">
+        <v>202.5</v>
+      </c>
+      <c r="C95" s="3">
+        <v>98.158929999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B96" s="3">
+        <v>203.5</v>
+      </c>
+      <c r="C96" s="3">
+        <v>99.64282</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97" s="3">
+        <v>204.5</v>
+      </c>
+      <c r="C97" s="3">
+        <v>101.14913</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" s="3">
+        <v>205.5</v>
+      </c>
+      <c r="C98" s="3">
+        <v>102.67821000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99" s="3">
+        <v>206.5</v>
+      </c>
+      <c r="C99" s="3">
+        <v>104.23041000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" s="3">
+        <v>207.5</v>
+      </c>
+      <c r="C100" s="3">
+        <v>105.80607999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B101" s="3">
+        <v>208.5</v>
+      </c>
+      <c r="C101" s="3">
+        <v>107.40555999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B102" s="3">
+        <v>209.5</v>
+      </c>
+      <c r="C102" s="3">
+        <v>109.02923</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103" s="3">
+        <v>210.5</v>
+      </c>
+      <c r="C103" s="3">
+        <v>110.67744</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B104" s="3">
+        <v>211.5</v>
+      </c>
+      <c r="C104" s="3">
+        <v>112.35056</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B105" s="3">
+        <v>212.5</v>
+      </c>
+      <c r="C105" s="3">
+        <v>114.04898</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" s="3">
+        <v>213.5</v>
+      </c>
+      <c r="C106" s="3">
+        <v>115.77307</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="3">
+        <v>214.5</v>
+      </c>
+      <c r="C107" s="3">
+        <v>117.52323</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108" s="3">
+        <v>215.5</v>
+      </c>
+      <c r="C108" s="3">
+        <v>119.29985000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109" s="3">
+        <v>216.5</v>
+      </c>
+      <c r="C109" s="3">
+        <v>121.10332</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110" s="3">
+        <v>217.5</v>
+      </c>
+      <c r="C110" s="3">
+        <v>122.93405</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B111" s="3">
+        <v>218.5</v>
+      </c>
+      <c r="C111" s="3">
+        <v>124.79246000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B112" s="3">
+        <v>219.5</v>
+      </c>
+      <c r="C112" s="3">
+        <v>126.67897000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B113" s="3">
+        <v>220.5</v>
+      </c>
+      <c r="C113" s="3">
+        <v>128.59398999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B114" s="3">
+        <v>221.5</v>
+      </c>
+      <c r="C114" s="3">
+        <v>130.53796</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115" s="3">
+        <v>222.5</v>
+      </c>
+      <c r="C115" s="3">
+        <v>132.51132000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B116" s="3">
+        <v>223.5</v>
+      </c>
+      <c r="C116" s="3">
+        <v>134.51451</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B117" s="3">
+        <v>224.5</v>
+      </c>
+      <c r="C117" s="3">
+        <v>136.54799</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B118" s="3">
+        <v>225.5</v>
+      </c>
+      <c r="C118" s="3">
+        <v>138.6122</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B119" s="3">
+        <v>226.5</v>
+      </c>
+      <c r="C119" s="3">
+        <v>140.70761999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B120" s="3">
+        <v>227.5</v>
+      </c>
+      <c r="C120" s="3">
+        <v>142.83471</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121" s="3">
+        <v>228.5</v>
+      </c>
+      <c r="C121" s="3">
+        <v>144.99396999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B122" s="3">
+        <v>229.5</v>
+      </c>
+      <c r="C122" s="3">
+        <v>147.18585999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B123" s="3">
+        <v>230.5</v>
+      </c>
+      <c r="C123" s="3">
+        <v>149.41088999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B124" s="3">
+        <v>231.5</v>
+      </c>
+      <c r="C124" s="3">
+        <v>151.66954999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B125" s="3">
+        <v>232.5</v>
+      </c>
+      <c r="C125" s="3">
+        <v>153.96235999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B126" s="3">
+        <v>233.5</v>
+      </c>
+      <c r="C126" s="3">
+        <v>156.28982999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B127" s="3">
+        <v>234.5</v>
+      </c>
+      <c r="C127" s="3">
+        <v>158.65248</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128" s="3">
+        <v>235.5</v>
+      </c>
+      <c r="C128" s="3">
+        <v>161.05085</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B129" s="3">
+        <v>236.5</v>
+      </c>
+      <c r="C129" s="3">
+        <v>163.48548</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B130" s="3">
+        <v>237.5</v>
+      </c>
+      <c r="C130" s="3">
+        <v>165.95690999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B131" s="3">
+        <v>238.5</v>
+      </c>
+      <c r="C131" s="3">
+        <v>168.46571</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B132" s="3">
+        <v>239.5</v>
+      </c>
+      <c r="C132" s="3">
+        <v>171.01241999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B133" s="3">
+        <v>240.5</v>
+      </c>
+      <c r="C133" s="3">
+        <v>173.59764000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B134" s="3">
+        <v>241.5</v>
+      </c>
+      <c r="C134" s="3">
+        <v>176.22193999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B135" s="3">
+        <v>242.5</v>
+      </c>
+      <c r="C135" s="3">
+        <v>178.88591</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B136" s="3">
+        <v>243.5</v>
+      </c>
+      <c r="C136" s="3">
+        <v>181.59014999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B137" s="3">
+        <v>244.5</v>
+      </c>
+      <c r="C137" s="3">
+        <v>184.33527000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B138" s="3">
+        <v>245.5</v>
+      </c>
+      <c r="C138" s="3">
+        <v>187.12189000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B139" s="3">
+        <v>246.5</v>
+      </c>
+      <c r="C139" s="3">
+        <v>189.95063999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B140" s="3">
+        <v>247.5</v>
+      </c>
+      <c r="C140" s="3">
+        <v>192.82214999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B141" s="3">
+        <v>248.5</v>
+      </c>
+      <c r="C141" s="3">
+        <v>195.73706999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B142" s="3">
+        <v>249.5</v>
+      </c>
+      <c r="C142" s="3">
+        <v>198.69605000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143" s="3">
+        <v>250.5</v>
+      </c>
+      <c r="C143" s="3">
+        <v>201.69977</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
len-wei by 5cm also included
</commit_message>
<xml_diff>
--- a/Length Weight/TTR_LengthWeight.xlsx
+++ b/Length Weight/TTR_LengthWeight.xlsx
@@ -550,10 +550,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B143"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -561,244 +561,418 @@
     <col min="1" max="2" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <v>110.5</v>
       </c>
       <c r="B3" s="3">
         <v>24.685580000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3">
+        <v>110.5</v>
+      </c>
+      <c r="E3">
+        <v>24.685580000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>111.5</v>
       </c>
       <c r="B4" s="3">
         <v>25.058759999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="D4">
+        <v>115.5</v>
+      </c>
+      <c r="E4">
+        <v>26.608730000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>112.5</v>
       </c>
       <c r="B5" s="3">
         <v>25.437570000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="D5">
+        <v>120.5</v>
+      </c>
+      <c r="E5">
+        <v>28.681699999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <v>113.5</v>
       </c>
       <c r="B6" s="3">
         <v>25.822120000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="D6">
+        <v>125.5</v>
+      </c>
+      <c r="E6">
+        <v>30.916170000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>114.5</v>
       </c>
       <c r="B7" s="3">
         <v>26.21247</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="D7">
+        <v>130.5</v>
+      </c>
+      <c r="E7">
+        <v>33.324719999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <v>115.5</v>
       </c>
       <c r="B8" s="3">
         <v>26.608730000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="D8">
+        <v>135.5</v>
+      </c>
+      <c r="E8">
+        <v>35.920909999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>116.5</v>
       </c>
       <c r="B9" s="3">
         <v>27.01098</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="D9">
+        <v>140.5</v>
+      </c>
+      <c r="E9">
+        <v>38.719349999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>117.5</v>
       </c>
       <c r="B10" s="3">
         <v>27.4193</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="D10">
+        <v>145.5</v>
+      </c>
+      <c r="E10">
+        <v>41.735810000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>118.5</v>
       </c>
       <c r="B11" s="3">
         <v>27.83381</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="D11">
+        <v>150.5</v>
+      </c>
+      <c r="E11">
+        <v>44.987270000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <v>119.5</v>
       </c>
       <c r="B12" s="3">
         <v>28.254570000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="D12">
+        <v>155.5</v>
+      </c>
+      <c r="E12">
+        <v>48.492040000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>120.5</v>
       </c>
       <c r="B13" s="3">
         <v>28.681699999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="D13">
+        <v>160.5</v>
+      </c>
+      <c r="E13">
+        <v>52.269849999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <v>121.5</v>
       </c>
       <c r="B14" s="3">
         <v>29.115290000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="D14">
+        <v>165.5</v>
+      </c>
+      <c r="E14">
+        <v>56.341970000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <v>122.5</v>
       </c>
       <c r="B15" s="3">
         <v>29.555430000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="D15">
+        <v>170.5</v>
+      </c>
+      <c r="E15">
+        <v>60.73133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <v>123.5</v>
       </c>
       <c r="B16" s="3">
         <v>30.002220000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="D16">
+        <v>175.5</v>
+      </c>
+      <c r="E16">
+        <v>65.462649999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="3">
         <v>124.5</v>
       </c>
       <c r="B17" s="3">
         <v>30.455770000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="D17">
+        <v>180.5</v>
+      </c>
+      <c r="E17">
+        <v>70.562569999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="3">
         <v>125.5</v>
       </c>
       <c r="B18" s="3">
         <v>30.916170000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="D18">
+        <v>185.5</v>
+      </c>
+      <c r="E18">
+        <v>76.059799999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="3">
         <v>126.5</v>
       </c>
       <c r="B19" s="3">
         <v>31.38353</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="D19">
+        <v>190.5</v>
+      </c>
+      <c r="E19">
+        <v>81.985290000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="3">
         <v>127.5</v>
       </c>
       <c r="B20" s="3">
         <v>31.857959999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="D20">
+        <v>195.5</v>
+      </c>
+      <c r="E20">
+        <v>88.372420000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="3">
         <v>128.5</v>
       </c>
       <c r="B21" s="3">
         <v>32.339570000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="D21">
+        <v>200.5</v>
+      </c>
+      <c r="E21">
+        <v>95.257140000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="3">
         <v>129.5</v>
       </c>
       <c r="B22" s="3">
         <v>32.828449999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="D22">
+        <v>205.5</v>
+      </c>
+      <c r="E22">
+        <v>102.67821000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="3">
         <v>130.5</v>
       </c>
       <c r="B23" s="3">
         <v>33.324719999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="D23">
+        <v>210.5</v>
+      </c>
+      <c r="E23">
+        <v>110.67744</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="3">
         <v>131.5</v>
       </c>
       <c r="B24" s="3">
         <v>33.828490000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="D24">
+        <v>215.5</v>
+      </c>
+      <c r="E24">
+        <v>119.29985000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="3">
         <v>132.5</v>
       </c>
       <c r="B25" s="3">
         <v>34.339880000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="D25">
+        <v>220.5</v>
+      </c>
+      <c r="E25">
+        <v>128.59398999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="3">
         <v>133.5</v>
       </c>
       <c r="B26" s="3">
         <v>34.859000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="D26">
+        <v>225.5</v>
+      </c>
+      <c r="E26">
+        <v>138.6122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="3">
         <v>134.5</v>
       </c>
       <c r="B27" s="3">
         <v>35.38597</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="D27">
+        <v>230.5</v>
+      </c>
+      <c r="E27">
+        <v>149.41088999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="3">
         <v>135.5</v>
       </c>
       <c r="B28" s="3">
         <v>35.920909999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="D28">
+        <v>235.5</v>
+      </c>
+      <c r="E28">
+        <v>161.05085</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="3">
         <v>136.5</v>
       </c>
       <c r="B29" s="3">
         <v>36.463929999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="D29">
+        <v>240.5</v>
+      </c>
+      <c r="E29">
+        <v>173.59764000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="3">
         <v>137.5</v>
       </c>
       <c r="B30" s="3">
         <v>37.015160000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="D30">
+        <v>245.5</v>
+      </c>
+      <c r="E30">
+        <v>187.12189000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="3">
         <v>138.5</v>
       </c>
       <c r="B31" s="3">
         <v>37.574719999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="D31">
+        <v>250.5</v>
+      </c>
+      <c r="E31">
+        <v>201.69977</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="3">
         <v>139.5</v>
       </c>

</xml_diff>